<commit_message>
Update Excel Download with SSZ Logo
</commit_message>
<xml_diff>
--- a/Titelblatt.xlsx
+++ b/Titelblatt.xlsx
@@ -5,7 +5,7 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="O:\Projekte\Bodenpreise\6_Shiny\LIMAneu\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="O:\Projekte\Bodenpreise\6_Shiny\LIMA_2.0\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="68">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="67">
   <si>
     <t>Napfgasse 6, 8022 Zürich</t>
   </si>
@@ -228,9 +228,6 @@
   </si>
   <si>
     <t>Preis pro Quadratmeter Wohnungsfläche bei Stockwerkeigentumskäufen</t>
-  </si>
-  <si>
-    <t>Statistik Stadt Zürich</t>
   </si>
 </sst>
 </file>
@@ -624,10 +621,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E12"/>
+  <dimension ref="A1:E11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A10" sqref="A10"/>
+      <selection activeCell="A2" sqref="A2:XFD2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -654,47 +651,42 @@
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
-        <v>67</v>
+        <v>0</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A6" s="1" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="D8" s="1" t="s">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="D7" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="E8" s="1" t="s">
+      <c r="E7" s="1" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A10" s="1" t="s">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A9" s="1" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A12" s="1" t="s">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A11" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="B12" s="1" t="s">
+      <c r="B11" s="1" t="s">
         <v>15</v>
       </c>
     </row>

</xml_diff>